<commit_message>
CWL attribute included into form sheets
</commit_message>
<xml_diff>
--- a/scratch/test_files/test_upload.input_form.xlsx
+++ b/scratch/test_files/test_upload.input_form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3a4525276f4ee0f6/home/CWLab/scratch/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{F1B1D056-01CD-466C-B34A-194EE04D9027}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{B0C57837-E307-40AC-840D-04EF58B8C43D}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="8_{F1B1D056-01CD-466C-B34A-194EE04D9027}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{3DA0F733-0E37-4B1C-A340-BBD579EF2ADB}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="global single values" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t># type: param | format: wide | param: fastq1 | run_id_param: run_id_fastq1</t>
   </si>
   <si>
-    <t># type: config</t>
-  </si>
-  <si>
     <t>parameter_name</t>
   </si>
   <si>
@@ -253,6 +250,9 @@
   </si>
   <si>
     <t>fq</t>
+  </si>
+  <si>
+    <t># CWL: ATAC-seq.cwl| type: config</t>
   </si>
 </sst>
 </file>
@@ -610,7 +610,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -618,7 +618,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -634,7 +634,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -675,18 +675,18 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -725,7 +725,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3">
         <v>73</v>
@@ -736,7 +736,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4">
         <v>74</v>
@@ -747,7 +747,7 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5">
         <v>75</v>
@@ -792,13 +792,13 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
         <v>66</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>67</v>
-      </c>
-      <c r="D3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -806,13 +806,13 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
         <v>69</v>
       </c>
-      <c r="C4" t="s">
-        <v>70</v>
-      </c>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -820,13 +820,13 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
         <v>72</v>
       </c>
-      <c r="C5" t="s">
-        <v>73</v>
-      </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -839,7 +839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
@@ -869,13 +869,13 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -883,13 +883,13 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -897,13 +897,13 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -915,86 +915,86 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>24</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>25</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>26</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>27</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>28</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>29</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>30</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>31</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>32</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>33</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>34</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>35</v>
-      </c>
-      <c r="P2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
         <v>37</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="C3" t="s">
-        <v>39</v>
-      </c>
       <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
         <v>40</v>
       </c>
-      <c r="E3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" t="s">
-        <v>41</v>
-      </c>
       <c r="P3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -1002,19 +1002,19 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -1022,48 +1022,48 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
         <v>43</v>
       </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>44</v>
       </c>
-      <c r="H5" t="s">
-        <v>45</v>
-      </c>
       <c r="P5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
         <v>46</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" t="s">
         <v>47</v>
       </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" t="s">
-        <v>48</v>
-      </c>
       <c r="P6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -1071,19 +1071,19 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -1091,22 +1091,22 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -1114,22 +1114,22 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" t="s">
         <v>49</v>
       </c>
-      <c r="C9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" t="s">
-        <v>50</v>
-      </c>
       <c r="P9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -1137,22 +1137,22 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -1160,19 +1160,19 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -1180,19 +1180,19 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -1200,42 +1200,42 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
         <v>53</v>
       </c>
-      <c r="B14" t="s">
-        <v>54</v>
-      </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -1243,39 +1243,39 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>